<commit_message>
Reorganized sections of introduction
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Potential-Research-Questions-by-Units-of-Analysis_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Potential-Research-Questions-by-Units-of-Analysis_v00.xlsx
@@ -438,8 +438,41 @@
     <t xml:space="preserve">Potential Research Question(s):  </t>
   </si>
   <si>
+    <t>Demand-side technology transfer decision makers use a decision premise that a technology has to have attained a minimum maturity level that is higher than the average maturity level of technologies available from universities.</t>
+  </si>
+  <si>
+    <t>In 80 percent of the cases, the demand-side technology transfer decision maker used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies available from universities.</t>
+  </si>
+  <si>
+    <t>In 80 percent of the cases, the demand-side technology transfer decision maker used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies patented by universities.</t>
+  </si>
+  <si>
+    <t>When making decisions about whether to acquire a technology, do most demand-side technology transfer decision makers use a decision premise that a technology must have a minimum maturity level that happens to be higher than the typical maturity level of technologies available from universities?</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>8d</t>
+  </si>
+  <si>
+    <t>8e</t>
+  </si>
+  <si>
+    <t>9c</t>
+  </si>
+  <si>
+    <t>10a</t>
+  </si>
+  <si>
+    <t>10b</t>
+  </si>
+  <si>
+    <t>Is technology maturity level part of the reason that a low percentage of technologies derived from federally-funded research and development conducted by U.S. universities are transferred to the private sector for use that benefits the public interest?</t>
+  </si>
+  <si>
     <r>
-      <t>R</t>
+      <t>Q</t>
     </r>
     <r>
       <rPr>
@@ -460,7 +493,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> through R</t>
+      <t xml:space="preserve"> through Q</t>
     </r>
     <r>
       <rPr>
@@ -483,39 +516,6 @@
       </rPr>
       <t xml:space="preserve"> (See table on units of analysis)</t>
     </r>
-  </si>
-  <si>
-    <t>Demand-side technology transfer decision makers use a decision premise that a technology has to have attained a minimum maturity level that is higher than the average maturity level of technologies available from universities.</t>
-  </si>
-  <si>
-    <t>In 80 percent of the cases, the demand-side technology transfer decision maker used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies available from universities.</t>
-  </si>
-  <si>
-    <t>In 80 percent of the cases, the demand-side technology transfer decision maker used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies patented by universities.</t>
-  </si>
-  <si>
-    <t>When making decisions about whether to acquire a technology, do most demand-side technology transfer decision makers use a decision premise that a technology must have a minimum maturity level that happens to be higher than the typical maturity level of technologies available from universities?</t>
-  </si>
-  <si>
-    <t>6c</t>
-  </si>
-  <si>
-    <t>8d</t>
-  </si>
-  <si>
-    <t>8e</t>
-  </si>
-  <si>
-    <t>9c</t>
-  </si>
-  <si>
-    <t>10a</t>
-  </si>
-  <si>
-    <t>10b</t>
-  </si>
-  <si>
-    <t>Is technology maturity level part of the reason that a low percentage of technologies derived from federally-funded research and development conducted by U.S. universities are transferred to the private sector for use that benefits the public interest?</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1043,8 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>R</a:t>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Q</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
@@ -1097,8 +1097,8 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>R</a:t>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Q</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
@@ -1151,8 +1151,8 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>R</a:t>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Q</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
@@ -1205,8 +1205,8 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>R</a:t>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Q</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
@@ -1259,8 +1259,8 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>R</a:t>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Q</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
@@ -1313,8 +1313,8 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>R</a:t>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Q</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
@@ -1766,7 +1766,7 @@
         <v>95</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
@@ -1824,7 +1824,7 @@
         <v>98</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
@@ -2153,11 +2153,11 @@
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O8" s="13">
         <v>21</v>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
@@ -2188,11 +2188,11 @@
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M9" s="12"/>
       <c r="N9" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O9" s="13">
         <v>22</v>
@@ -2200,14 +2200,14 @@
     </row>
     <row r="10" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
@@ -2223,11 +2223,11 @@
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O10" s="13">
         <v>23</v>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>34</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="17" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>34</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="20" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>34</v>
@@ -2589,7 +2589,7 @@
     </row>
     <row r="21" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>34</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="22" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>34</v>

</xml_diff>